<commit_message>
Program-Template.xlsx: update new template
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/Program-Template.xlsx
+++ b/src/main/resources/templates/Program-Template.xlsx
@@ -5,31 +5,20 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\HiepNH\Documents\_FPT\2023\Spring\OJT\FA-Training-System\fa-training-system\src\main\resources\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\HiepNH\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80538833-D7A2-4B22-AEDD-F37A0DFC7660}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8902F852-F5ED-415C-849D-6358A07DF4D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{EC8A8B09-C0A3-4AB7-B2FE-92915CEE8C22}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Program list" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -41,25 +30,25 @@
     <t>Program Name</t>
   </si>
   <si>
-    <t>This is program name</t>
-  </si>
-  <si>
     <t>Activated</t>
   </si>
   <si>
-    <t>This is program name 2</t>
-  </si>
-  <si>
-    <t>FAB473,NGK437,HNF753</t>
-  </si>
-  <si>
-    <t>HNF753,LKI657</t>
-  </si>
-  <si>
     <t>Syllabus Codes</t>
   </si>
   <si>
     <t>Program ID</t>
+  </si>
+  <si>
+    <t>SAP Development Foundation</t>
+  </si>
+  <si>
+    <t>6AIV3,4F4Q0</t>
+  </si>
+  <si>
+    <t>Cloud Programming Foundation</t>
+  </si>
+  <si>
+    <t>2724D,46NM9,5H07V</t>
   </si>
 </sst>
 </file>
@@ -101,10 +90,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -418,62 +406,56 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1743C78-E38C-434E-8EC0-3B314D8F4854}">
-  <dimension ref="A1:D4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.140625" customWidth="1"/>
+    <col min="2" max="2" width="29.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="28.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="2" t="b">
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="b">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>